<commit_message>
Gesamtinvestitionskosten UST implementiert + Scrollbar hinzugefügt
Weitere TO Do's für GIK:
-Inputvalisierung:
Nur numerische Variablen sollten erlaubt sein;
Bei dem Input soll 0,7 in 0.7 konvertiert werden.
70% ebenfalls 0.7. Momentan funktioniert nur die Schreibweise 0.7

Herr Wala fragen, ob Inputs so korrekt sind
</commit_message>
<xml_diff>
--- a/SEPJ-Rechnungen.xlsx
+++ b/SEPJ-Rechnungen.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\src\main\resources\com\example\financingtool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\IdeaProjects\FinancingTool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B301BBC2-0550-4CBE-9487-1CE8D7E11D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB75F70-A069-46E0-8AA3-760964373476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{4C9598BD-5712-4F7A-AC8E-F76386525838}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -777,8 +777,8 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="n">
-        <v>270.0</v>
+      <c r="B2" s="1">
+        <v>270</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -923,19 +923,19 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.1328125" collapsed="true"/>
-    <col min="2" max="3" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.86328125" collapsed="true"/>
+    <col min="1" max="1" width="31.1328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.86328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="8" t="n">
-        <v>100.0</v>
+      <c r="A1" s="8">
+        <v>100</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>15</v>
@@ -1311,10 +1311,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.59765625" collapsed="true"/>
-    <col min="2" max="3" customWidth="true" width="10.73046875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="21.3984375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
+    <col min="1" max="1" width="21.59765625" customWidth="1" collapsed="1"/>
+    <col min="2" max="3" width="10.73046875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="21.3984375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -1462,11 +1462,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="42.86328125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.1328125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.86328125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.73046875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.1328125" collapsed="true"/>
+    <col min="1" max="1" width="42.86328125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.1328125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.86328125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.73046875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.1328125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.55000000000000004">
@@ -1937,23 +1937,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101009729EB743038154A9A59E0B356D92C1D" ma:contentTypeVersion="7" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="2a57c8d8c641ac19acee86c7c4b3ca99">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5a8965bb-c16f-4a6f-82bb-93d665d6df35" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7f73fa18acbcaf29007fba3bb0351da" ns3:_="">
     <xsd:import namespace="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
@@ -2117,25 +2100,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="5a8965bb-c16f-4a6f-82bb-93d665d6df35" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95D91BE8-21EF-4DB4-BD5E-4B3C53A56A32}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2151,4 +2133,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43C913E0-75E0-4CB8-A616-4F388A0CD568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9F7DD2DD-E6A0-4AD2-8B5B-E10BEBC466C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="5a8965bb-c16f-4a6f-82bb-93d665d6df35"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>